<commit_message>
cambios en los tikets para imprimir y algunas urls
</commit_message>
<xml_diff>
--- a/cajas-diarias/caja-2023-09-05.xlsx
+++ b/cajas-diarias/caja-2023-09-05.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -453,9 +453,128 @@
         <v>DEBITO</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>ESTAMPA</v>
+      </c>
+      <c r="B4" t="str">
+        <v>20000</v>
+      </c>
+      <c r="C4" t="str">
+        <v>GATO</v>
+      </c>
+      <c r="D4" t="str">
+        <v>15</v>
+      </c>
+      <c r="E4" t="str">
+        <v>CREDITO</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>NUTRIBON</v>
+      </c>
+      <c r="B5" t="str">
+        <v>8300</v>
+      </c>
+      <c r="C5" t="str">
+        <v>PERRO</v>
+      </c>
+      <c r="D5" t="str">
+        <v>20</v>
+      </c>
+      <c r="E5" t="str">
+        <v>TRANSFERENCIA</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>DOGUI</v>
+      </c>
+      <c r="B6" t="str">
+        <v>8000</v>
+      </c>
+      <c r="C6" t="str">
+        <v>PERRO</v>
+      </c>
+      <c r="D6" t="str">
+        <v>21</v>
+      </c>
+      <c r="E6" t="str">
+        <v>TRANSFERENCIA</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>NUTRIBON</v>
+      </c>
+      <c r="B7" t="str">
+        <v>13333</v>
+      </c>
+      <c r="C7" t="str">
+        <v>GATO</v>
+      </c>
+      <c r="D7" t="str">
+        <v>20</v>
+      </c>
+      <c r="E7" t="str">
+        <v>EFECTIVO</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>NUTRIBON</v>
+      </c>
+      <c r="B8" t="str">
+        <v>5100</v>
+      </c>
+      <c r="C8" t="str">
+        <v>PERRO</v>
+      </c>
+      <c r="D8" t="str">
+        <v>20</v>
+      </c>
+      <c r="E8" t="str">
+        <v>EFECTIVO</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>DOGUI</v>
+      </c>
+      <c r="B9" t="str">
+        <v>499</v>
+      </c>
+      <c r="C9" t="str">
+        <v>PERRO</v>
+      </c>
+      <c r="D9" t="str">
+        <v>2</v>
+      </c>
+      <c r="E9" t="str">
+        <v>EFECTIVO</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>JHOLA</v>
+      </c>
+      <c r="B10" t="str">
+        <v>5100</v>
+      </c>
+      <c r="C10" t="str">
+        <v>PERRO</v>
+      </c>
+      <c r="D10" t="str">
+        <v>20</v>
+      </c>
+      <c r="E10" t="str">
+        <v>EFECTIVO</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>